<commit_message>
Aggiunto bot telegram e controllo per input vuoto
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -1,98 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\apala\Desktop\PRova excel python\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6530735F-D23F-4F0B-9609-8359CEAE25F0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Database" sheetId="1" r:id="rId1"/>
-    <sheet name="Nk" sheetId="2" r:id="rId2"/>
+    <sheet name="Database" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Nk" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t xml:space="preserve">NOMI: </t>
-  </si>
-  <si>
-    <t>Descrizione</t>
-  </si>
-  <si>
-    <t>Armadio</t>
-  </si>
-  <si>
-    <t>Sedia</t>
-  </si>
-  <si>
-    <t>Rospo</t>
-  </si>
-  <si>
-    <t>Tastiera</t>
-  </si>
-  <si>
-    <t>Ginepro</t>
-  </si>
-  <si>
-    <t>Comodino</t>
-  </si>
-  <si>
-    <t>Salve</t>
-  </si>
-  <si>
-    <t>Ciao</t>
-  </si>
-  <si>
-    <t>Comdoino</t>
-  </si>
-  <si>
-    <t>Comdo</t>
-  </si>
-  <si>
-    <t>Mobile costituito essenzialmente di due fiancate verticali a sostegno di scaffali o di liste trasversali per attaccapanni e chiuso anteriormente da sportelli (detti anche ante ) che possono, considerati singolarmente o a coppia, corrispondere ad altrettanti scomparti all'interno.</t>
-  </si>
-  <si>
-    <t>Mobile destinato a offrire appoggio alla persona seduta, essenzialmente costituito di un piano sostenuto da piedi o gambe in numero variabile ed eventualmente da parti per l'appoggio delle braccia ( braccioli ) o del dorso ( spalliera )</t>
-  </si>
-  <si>
-    <t>Nome com. degli Anfibi Anuri dei Bufonidi, part. del Bufo bufo, dal corpo tozzo e appiattito, con pelle di colore variabile dal bruno al verde olivastro, ricca di ghiandole secernenti una sostanza irritante; la notte va a caccia di insetti, crostacei, molluschi e talvolta anche di piccoli mammiferi; vive nell'acqua solo nel periodo dell'accoppiamento (febbraio-marzo).</t>
-  </si>
-  <si>
-    <t>Il complesso dei tasti di una macchina da scrivere, di una calcolatrice, di una telescrivente, di un elaboratore elettronico o di un suo terminale.</t>
-  </si>
-  <si>
-    <t>Arbusto delle Cupressacee ( Iuniperus communis ), con corteccia grigio-rossastra, foglie lineari, rigide e pungenti, persistenti, in verticilli di tre foglie alterne, frutti di colore azzurro (detti com. coccole ).</t>
-  </si>
-  <si>
-    <t>Armadietto dell'altezza di un tavolino, installato presso il letto.</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -111,21 +47,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -413,104 +408,191 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-    </row>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NOMI: </t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Descrizione</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Armadio</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Mobile costituito essenzialmente di due fiancate verticali a sostegno di scaffali o di liste trasversali per attaccapanni e chiuso anteriormente da sportelli (detti anche ante ) che possono, considerati singolarmente o a coppia, corrispondere ad altrettanti scomparti all'interno.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Sedia</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Mobile destinato a offrire appoggio alla persona seduta, essenzialmente costituito di un piano sostenuto da piedi o gambe in numero variabile ed eventualmente da parti per l'appoggio delle braccia ( braccioli ) o del dorso ( spalliera )</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Rospo</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Nome com. degli Anfibi Anuri dei Bufonidi, part. del Bufo bufo, dal corpo tozzo e appiattito, con pelle di colore variabile dal bruno al verde olivastro, ricca di ghiandole secernenti una sostanza irritante; la notte va a caccia di insetti, crostacei, molluschi e talvolta anche di piccoli mammiferi; vive nell'acqua solo nel periodo dell'accoppiamento (febbraio-marzo).</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Tastiera</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Il complesso dei tasti di una macchina da scrivere, di una calcolatrice, di una telescrivente, di un elaboratore elettronico o di un suo terminale.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Ginepro</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Arbusto delle Cupressacee ( Iuniperus communis ), con corteccia grigio-rossastra, foglie lineari, rigide e pungenti, persistenti, in verticilli di tre foglie alterne, frutti di colore azzurro (detti com. coccole ).</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Comodino</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Armadietto dell'altezza di un tavolino, installato presso il letto.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Salve</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Ciao</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Comdoino</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Comdo</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Lumaca</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Squalo</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>/definisci</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>{'id': 422619671, 'first_name': 'Alessandro', 'is_bot': False, 'language_code': 'it'}</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Sucaaaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Ciaaaaaa</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiunto supporto per parole composte!
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
@@ -595,6 +595,62 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Porca</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Gay</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Arcobaleno</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Dio</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Comodinodio</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Start</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Pisellino</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Porco spino</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Cambiamento da /definisci a /def
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" state="visible" r:id="rId1"/>
@@ -413,10 +413,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -505,7 +505,19 @@
         </is>
       </c>
     </row>
-    <row r="8"/>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Cacca</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Escremento -- ZATINI</t>
+        </is>
+      </c>
+    </row>
+    <row r="9"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -517,10 +529,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:A25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -651,6 +663,55 @@
         </is>
       </c>
     </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Porca madonna laida</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Abuso di bambini canguro</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Bocca</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Stocazzo</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Cacca</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Suuucaaaaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Porcoddiomaialebastardonegrobruttoinfame</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Aggiunta documentazione inserita su botFather
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -517,7 +517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
@@ -581,6 +581,13 @@
         </is>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Provola</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Aggiunto file con codice commentato
</commit_message>
<xml_diff>
--- a/DataBase.xlsx
+++ b/DataBase.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Database" sheetId="1" state="visible" r:id="rId1"/>
@@ -415,7 +415,7 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -517,10 +517,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -588,7 +588,57 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> antilope</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Antilope</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Barbagianni</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Pippo</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Fagiolo</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Aaaaaaaaaaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Aaaaaaaaaaaaaaaaaa</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" paperSize="9" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>